<commit_message>
Se agregan total producido y total defectos
</commit_message>
<xml_diff>
--- a/distribucion.xlsx
+++ b/distribucion.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Registro_defectos_SEHO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E2C6535-FDE1-462C-BAC9-5A61457182CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D501BC49-F73E-442D-A8F6-EC105866AA91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="6" xr2:uid="{C5A581BF-84BA-4755-84C9-6391AAA71289}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="5" xr2:uid="{C5A581BF-84BA-4755-84C9-6391AAA71289}"/>
   </bookViews>
   <sheets>
     <sheet name="Frame0" sheetId="2" r:id="rId1"/>
@@ -74,7 +74,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="553" uniqueCount="339">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="589" uniqueCount="371">
   <si>
     <t>FA08</t>
   </si>
@@ -652,9 +652,6 @@
     <t>TopDefectos:</t>
   </si>
   <si>
-    <t>TotalDefectos:</t>
-  </si>
-  <si>
     <t>%Defectos:</t>
   </si>
   <si>
@@ -1081,9 +1078,6 @@
     <t>button_16</t>
   </si>
   <si>
-    <t>button_17</t>
-  </si>
-  <si>
     <t>root_defect_frame0</t>
   </si>
   <si>
@@ -1091,6 +1085,108 @@
   </si>
   <si>
     <t>label_de_0</t>
+  </si>
+  <si>
+    <t>Cant.Defecto:</t>
+  </si>
+  <si>
+    <t>Row_9</t>
+  </si>
+  <si>
+    <t>Row_10</t>
+  </si>
+  <si>
+    <t>label_154</t>
+  </si>
+  <si>
+    <t>label_155</t>
+  </si>
+  <si>
+    <t>label_156</t>
+  </si>
+  <si>
+    <t>label_157</t>
+  </si>
+  <si>
+    <t>label_158</t>
+  </si>
+  <si>
+    <t>label_159</t>
+  </si>
+  <si>
+    <t>label_160</t>
+  </si>
+  <si>
+    <t>label_161</t>
+  </si>
+  <si>
+    <t>label_162</t>
+  </si>
+  <si>
+    <t>label_163</t>
+  </si>
+  <si>
+    <t>label_164</t>
+  </si>
+  <si>
+    <t>label_165</t>
+  </si>
+  <si>
+    <t>label_166</t>
+  </si>
+  <si>
+    <t>label_167</t>
+  </si>
+  <si>
+    <t>label_168</t>
+  </si>
+  <si>
+    <t>label_169</t>
+  </si>
+  <si>
+    <t>label_170</t>
+  </si>
+  <si>
+    <t>label_171</t>
+  </si>
+  <si>
+    <t>label_172</t>
+  </si>
+  <si>
+    <t>label_173</t>
+  </si>
+  <si>
+    <t>label_174</t>
+  </si>
+  <si>
+    <t>label_175</t>
+  </si>
+  <si>
+    <t>label_176</t>
+  </si>
+  <si>
+    <t>label_177</t>
+  </si>
+  <si>
+    <t>label_178</t>
+  </si>
+  <si>
+    <t>TotalDefect:</t>
+  </si>
+  <si>
+    <t>TotalProduc:</t>
+  </si>
+  <si>
+    <t>label_179</t>
+  </si>
+  <si>
+    <t>label_180</t>
+  </si>
+  <si>
+    <t>TopDefect:</t>
+  </si>
+  <si>
+    <t>Cant.Defect:</t>
   </si>
 </sst>
 </file>
@@ -1159,7 +1255,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="21">
+  <fills count="22">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1270,13 +1366,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF3737"/>
+        <fgColor rgb="FF0070C0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF0070C0"/>
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1447,12 +1549,6 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1483,13 +1579,13 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1501,8 +1597,14 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2668,18 +2770,18 @@
       <c r="A2" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="B2" s="42" t="s">
+      <c r="B2" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="42"/>
-      <c r="D2" s="42"/>
-      <c r="E2" s="42"/>
-      <c r="F2" s="42"/>
-      <c r="G2" s="42"/>
-      <c r="H2" s="42"/>
-      <c r="I2" s="42"/>
-      <c r="J2" s="42"/>
-      <c r="K2" s="42"/>
+      <c r="C2" s="40"/>
+      <c r="D2" s="40"/>
+      <c r="E2" s="40"/>
+      <c r="F2" s="40"/>
+      <c r="G2" s="40"/>
+      <c r="H2" s="40"/>
+      <c r="I2" s="40"/>
+      <c r="J2" s="40"/>
+      <c r="K2" s="40"/>
     </row>
     <row r="3" spans="1:11" ht="24" x14ac:dyDescent="0.4">
       <c r="A3" s="9" t="s">
@@ -2838,12 +2940,12 @@
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
-      <c r="E9" s="43" t="s">
+      <c r="E9" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="F9" s="43"/>
-      <c r="G9" s="43"/>
-      <c r="H9" s="43"/>
+      <c r="F9" s="41"/>
+      <c r="G9" s="41"/>
+      <c r="H9" s="41"/>
       <c r="I9" s="1"/>
       <c r="J9" s="2"/>
       <c r="K9" s="2"/>
@@ -2855,10 +2957,10 @@
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
-      <c r="E10" s="41"/>
-      <c r="F10" s="41"/>
-      <c r="G10" s="41"/>
-      <c r="H10" s="41"/>
+      <c r="E10" s="39"/>
+      <c r="F10" s="39"/>
+      <c r="G10" s="39"/>
+      <c r="H10" s="39"/>
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
       <c r="K10" s="1"/>
@@ -2902,18 +3004,18 @@
       <c r="A14" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="B14" s="42" t="s">
+      <c r="B14" s="40" t="s">
         <v>60</v>
       </c>
-      <c r="C14" s="42"/>
-      <c r="D14" s="42"/>
-      <c r="E14" s="42"/>
-      <c r="F14" s="42"/>
-      <c r="G14" s="42"/>
-      <c r="H14" s="42"/>
-      <c r="I14" s="42"/>
-      <c r="J14" s="42"/>
-      <c r="K14" s="42"/>
+      <c r="C14" s="40"/>
+      <c r="D14" s="40"/>
+      <c r="E14" s="40"/>
+      <c r="F14" s="40"/>
+      <c r="G14" s="40"/>
+      <c r="H14" s="40"/>
+      <c r="I14" s="40"/>
+      <c r="J14" s="40"/>
+      <c r="K14" s="40"/>
     </row>
     <row r="15" spans="1:11" ht="24" x14ac:dyDescent="0.4">
       <c r="A15" s="9" t="s">
@@ -3132,12 +3234,12 @@
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
-      <c r="E21" s="43" t="s">
+      <c r="E21" s="41" t="s">
         <v>130</v>
       </c>
-      <c r="F21" s="43"/>
-      <c r="G21" s="43"/>
-      <c r="H21" s="43"/>
+      <c r="F21" s="41"/>
+      <c r="G21" s="41"/>
+      <c r="H21" s="41"/>
       <c r="I21" s="1"/>
       <c r="J21" s="2"/>
       <c r="K21" s="2"/>
@@ -3149,12 +3251,12 @@
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
-      <c r="E22" s="41" t="s">
+      <c r="E22" s="39" t="s">
         <v>168</v>
       </c>
-      <c r="F22" s="41"/>
-      <c r="G22" s="41"/>
-      <c r="H22" s="41"/>
+      <c r="F22" s="39"/>
+      <c r="G22" s="39"/>
+      <c r="H22" s="39"/>
       <c r="I22" s="1"/>
       <c r="J22" s="1"/>
       <c r="K22" s="1"/>
@@ -3512,14 +3614,15 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D85BEB1E-8402-4209-AC46-FA5A75617005}">
-  <dimension ref="A1:AC32"/>
+  <dimension ref="A1:AC38"/>
   <sheetViews>
     <sheetView topLeftCell="A10" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+      <selection activeCell="N36" sqref="N36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="2" max="2" width="12" customWidth="1"/>
     <col min="17" max="25" width="11.5703125" customWidth="1"/>
     <col min="26" max="29" width="12.5703125" customWidth="1"/>
   </cols>
@@ -3569,1009 +3672,1177 @@
       </c>
     </row>
     <row r="2" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="15" t="s">
         <v>41</v>
       </c>
       <c r="B2" s="14"/>
       <c r="C2" s="23" t="s">
         <v>182</v>
       </c>
-      <c r="D2" s="31" t="s">
+      <c r="D2" s="29" t="s">
         <v>183</v>
       </c>
       <c r="E2" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="31" t="s">
+      <c r="F2" s="29" t="s">
         <v>184</v>
       </c>
       <c r="G2" s="23" t="s">
         <v>186</v>
       </c>
-      <c r="H2" s="31" t="s">
+      <c r="H2" s="29" t="s">
         <v>0</v>
       </c>
       <c r="I2" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="J2" s="31" t="s">
+      <c r="J2" s="29" t="s">
         <v>1</v>
       </c>
       <c r="K2" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="L2" s="31" t="s">
+      <c r="L2" s="29" t="s">
         <v>2</v>
       </c>
       <c r="M2" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="N2" s="31" t="s">
+      <c r="N2" s="29" t="s">
         <v>185</v>
       </c>
-      <c r="Q2" s="32" t="s">
+      <c r="Q2" s="30" t="s">
+        <v>296</v>
+      </c>
+      <c r="R2" s="31" t="s">
         <v>297</v>
       </c>
-      <c r="R2" s="33" t="s">
+      <c r="S2" s="31" t="s">
         <v>298</v>
       </c>
-      <c r="S2" s="33" t="s">
+      <c r="T2" s="31" t="s">
         <v>299</v>
       </c>
-      <c r="T2" s="33" t="s">
+      <c r="U2" s="31" t="s">
         <v>300</v>
       </c>
-      <c r="U2" s="33" t="s">
+      <c r="V2" s="31" t="s">
         <v>301</v>
       </c>
-      <c r="V2" s="33" t="s">
+      <c r="W2" s="31" t="s">
         <v>302</v>
       </c>
-      <c r="W2" s="33" t="s">
+      <c r="X2" s="31" t="s">
         <v>303</v>
       </c>
-      <c r="X2" s="33" t="s">
+      <c r="Y2" s="31" t="s">
         <v>304</v>
       </c>
-      <c r="Y2" s="33" t="s">
+      <c r="Z2" s="31" t="s">
         <v>305</v>
       </c>
-      <c r="Z2" s="33" t="s">
+      <c r="AA2" s="31" t="s">
         <v>306</v>
       </c>
-      <c r="AA2" s="33" t="s">
+      <c r="AB2" s="31" t="s">
         <v>307</v>
       </c>
-      <c r="AB2" s="33" t="s">
+      <c r="AC2" s="32" t="s">
         <v>308</v>
       </c>
-      <c r="AC2" s="34" t="s">
-        <v>309</v>
-      </c>
     </row>
     <row r="3" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="15" t="s">
         <v>53</v>
       </c>
       <c r="B3" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="28"/>
-      <c r="D3" s="29"/>
-      <c r="E3" s="28"/>
-      <c r="F3" s="29"/>
-      <c r="G3" s="28"/>
-      <c r="H3" s="29"/>
-      <c r="I3" s="28"/>
-      <c r="J3" s="29"/>
-      <c r="K3" s="28"/>
-      <c r="L3" s="29"/>
-      <c r="M3" s="28"/>
-      <c r="N3" s="29"/>
-      <c r="Q3" s="35" t="s">
+      <c r="C3" s="26"/>
+      <c r="D3" s="27"/>
+      <c r="E3" s="26"/>
+      <c r="F3" s="27"/>
+      <c r="G3" s="26"/>
+      <c r="H3" s="27"/>
+      <c r="I3" s="26"/>
+      <c r="J3" s="27"/>
+      <c r="K3" s="26"/>
+      <c r="L3" s="27"/>
+      <c r="M3" s="26"/>
+      <c r="N3" s="27"/>
+      <c r="Q3" s="33" t="s">
         <v>42</v>
       </c>
-      <c r="R3" s="36" t="s">
+      <c r="R3" s="34" t="s">
         <v>43</v>
       </c>
-      <c r="S3" s="36" t="s">
+      <c r="S3" s="34" t="s">
         <v>44</v>
       </c>
-      <c r="T3" s="36" t="s">
+      <c r="T3" s="34" t="s">
         <v>46</v>
       </c>
-      <c r="U3" s="36" t="s">
+      <c r="U3" s="34" t="s">
         <v>47</v>
       </c>
-      <c r="V3" s="36" t="s">
+      <c r="V3" s="34" t="s">
         <v>48</v>
       </c>
-      <c r="W3" s="36" t="s">
+      <c r="W3" s="34" t="s">
         <v>49</v>
       </c>
-      <c r="X3" s="36" t="s">
+      <c r="X3" s="34" t="s">
         <v>50</v>
       </c>
-      <c r="Y3" s="36" t="s">
+      <c r="Y3" s="34" t="s">
         <v>51</v>
       </c>
-      <c r="Z3" s="36" t="s">
+      <c r="Z3" s="34" t="s">
         <v>52</v>
       </c>
-      <c r="AA3" s="36" t="s">
+      <c r="AA3" s="34" t="s">
         <v>119</v>
       </c>
-      <c r="AB3" s="36" t="s">
+      <c r="AB3" s="34" t="s">
         <v>120</v>
       </c>
-      <c r="AC3" s="37" t="s">
+      <c r="AC3" s="35" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="4" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="15" t="s">
         <v>54</v>
       </c>
       <c r="B4" s="25" t="s">
         <v>187</v>
       </c>
-      <c r="C4" s="28"/>
-      <c r="D4" s="29"/>
-      <c r="E4" s="28"/>
-      <c r="F4" s="29"/>
-      <c r="G4" s="28"/>
-      <c r="H4" s="29"/>
-      <c r="I4" s="28"/>
-      <c r="J4" s="29"/>
-      <c r="K4" s="28"/>
-      <c r="L4" s="29"/>
-      <c r="M4" s="28"/>
-      <c r="N4" s="29"/>
+      <c r="C4" s="26"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="26"/>
+      <c r="F4" s="27"/>
+      <c r="G4" s="26"/>
+      <c r="H4" s="27"/>
+      <c r="I4" s="26"/>
+      <c r="J4" s="27"/>
+      <c r="K4" s="26"/>
+      <c r="L4" s="27"/>
+      <c r="M4" s="26"/>
+      <c r="N4" s="27"/>
     </row>
     <row r="5" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="15" t="s">
         <v>55</v>
       </c>
       <c r="B5" s="25" t="s">
         <v>188</v>
       </c>
-      <c r="C5" s="28"/>
-      <c r="D5" s="29"/>
-      <c r="E5" s="28"/>
-      <c r="F5" s="29"/>
-      <c r="G5" s="28"/>
-      <c r="H5" s="29"/>
-      <c r="I5" s="28"/>
-      <c r="J5" s="29"/>
-      <c r="K5" s="28"/>
-      <c r="L5" s="29"/>
-      <c r="M5" s="28"/>
-      <c r="N5" s="29"/>
+      <c r="C5" s="26"/>
+      <c r="D5" s="27"/>
+      <c r="E5" s="26"/>
+      <c r="F5" s="27"/>
+      <c r="G5" s="26"/>
+      <c r="H5" s="27"/>
+      <c r="I5" s="26"/>
+      <c r="J5" s="27"/>
+      <c r="K5" s="26"/>
+      <c r="L5" s="27"/>
+      <c r="M5" s="26"/>
+      <c r="N5" s="27"/>
     </row>
     <row r="6" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="15" t="s">
         <v>56</v>
       </c>
       <c r="B6" s="17"/>
-      <c r="C6" s="30" t="s">
+      <c r="C6" s="28" t="s">
         <v>189</v>
       </c>
-      <c r="D6" s="30" t="s">
+      <c r="D6" s="28" t="s">
         <v>189</v>
       </c>
-      <c r="E6" s="30" t="s">
+      <c r="E6" s="28" t="s">
         <v>189</v>
       </c>
-      <c r="F6" s="30" t="s">
+      <c r="F6" s="28" t="s">
         <v>189</v>
       </c>
-      <c r="G6" s="30" t="s">
+      <c r="G6" s="28" t="s">
         <v>189</v>
       </c>
-      <c r="H6" s="30" t="s">
+      <c r="H6" s="28" t="s">
         <v>189</v>
       </c>
-      <c r="I6" s="30" t="s">
+      <c r="I6" s="28" t="s">
         <v>189</v>
       </c>
-      <c r="J6" s="30" t="s">
+      <c r="J6" s="28" t="s">
         <v>189</v>
       </c>
-      <c r="K6" s="30" t="s">
+      <c r="K6" s="28" t="s">
         <v>189</v>
       </c>
-      <c r="L6" s="30" t="s">
+      <c r="L6" s="28" t="s">
         <v>189</v>
       </c>
-      <c r="M6" s="30" t="s">
+      <c r="M6" s="28" t="s">
         <v>189</v>
       </c>
-      <c r="N6" s="30" t="s">
+      <c r="N6" s="28" t="s">
         <v>189</v>
       </c>
     </row>
     <row r="7" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="B7" s="26" t="s">
+      <c r="B7" s="42" t="s">
         <v>190</v>
       </c>
-      <c r="C7" s="28"/>
-      <c r="D7" s="29"/>
-      <c r="E7" s="28"/>
-      <c r="F7" s="29"/>
-      <c r="G7" s="28"/>
-      <c r="H7" s="29"/>
-      <c r="I7" s="28"/>
-      <c r="J7" s="29"/>
-      <c r="K7" s="28"/>
-      <c r="L7" s="29"/>
-      <c r="M7" s="28"/>
-      <c r="N7" s="29"/>
+      <c r="C7" s="26"/>
+      <c r="D7" s="27"/>
+      <c r="E7" s="26"/>
+      <c r="F7" s="27"/>
+      <c r="G7" s="26"/>
+      <c r="H7" s="27"/>
+      <c r="I7" s="26"/>
+      <c r="J7" s="27"/>
+      <c r="K7" s="26"/>
+      <c r="L7" s="27"/>
+      <c r="M7" s="26"/>
+      <c r="N7" s="27"/>
     </row>
     <row r="8" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="B8" s="27" t="s">
-        <v>191</v>
-      </c>
-      <c r="C8" s="28"/>
-      <c r="D8" s="29"/>
-      <c r="E8" s="28"/>
-      <c r="F8" s="29"/>
-      <c r="G8" s="28"/>
-      <c r="H8" s="29"/>
-      <c r="I8" s="28"/>
-      <c r="J8" s="29"/>
-      <c r="K8" s="28"/>
-      <c r="L8" s="29"/>
-      <c r="M8" s="28"/>
-      <c r="N8" s="29"/>
+      <c r="B8" s="42" t="s">
+        <v>365</v>
+      </c>
+      <c r="C8" s="26"/>
+      <c r="D8" s="27"/>
+      <c r="E8" s="26"/>
+      <c r="F8" s="27"/>
+      <c r="G8" s="26"/>
+      <c r="H8" s="27"/>
+      <c r="I8" s="26"/>
+      <c r="J8" s="27"/>
+      <c r="K8" s="26"/>
+      <c r="L8" s="27"/>
+      <c r="M8" s="26"/>
+      <c r="N8" s="27"/>
     </row>
     <row r="9" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="B9" s="27" t="s">
-        <v>192</v>
-      </c>
-      <c r="C9" s="28"/>
-      <c r="D9" s="29"/>
-      <c r="E9" s="28"/>
-      <c r="F9" s="29"/>
-      <c r="G9" s="28"/>
-      <c r="H9" s="29"/>
-      <c r="I9" s="28"/>
-      <c r="J9" s="29"/>
-      <c r="K9" s="28"/>
-      <c r="L9" s="29"/>
-      <c r="M9" s="28"/>
-      <c r="N9" s="29"/>
+      <c r="B9" s="42" t="s">
+        <v>366</v>
+      </c>
+      <c r="C9" s="26"/>
+      <c r="D9" s="27"/>
+      <c r="E9" s="26"/>
+      <c r="F9" s="27"/>
+      <c r="G9" s="26"/>
+      <c r="H9" s="27"/>
+      <c r="I9" s="26"/>
+      <c r="J9" s="27"/>
+      <c r="K9" s="26"/>
+      <c r="L9" s="27"/>
+      <c r="M9" s="26"/>
+      <c r="N9" s="27"/>
     </row>
     <row r="10" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>159</v>
       </c>
-      <c r="B10" s="27" t="s">
-        <v>193</v>
-      </c>
-      <c r="C10" s="28"/>
-      <c r="D10" s="29"/>
-      <c r="E10" s="28"/>
-      <c r="F10" s="29"/>
-      <c r="G10" s="28"/>
-      <c r="H10" s="29"/>
-      <c r="I10" s="28"/>
-      <c r="J10" s="29"/>
-      <c r="K10" s="28"/>
-      <c r="L10" s="29"/>
-      <c r="M10" s="28"/>
-      <c r="N10" s="29"/>
+      <c r="B10" s="43" t="s">
+        <v>191</v>
+      </c>
+      <c r="C10" s="26"/>
+      <c r="D10" s="27"/>
+      <c r="E10" s="26"/>
+      <c r="F10" s="27"/>
+      <c r="G10" s="26"/>
+      <c r="H10" s="27"/>
+      <c r="I10" s="26"/>
+      <c r="J10" s="27"/>
+      <c r="K10" s="26"/>
+      <c r="L10" s="27"/>
+      <c r="M10" s="26"/>
+      <c r="N10" s="27"/>
+    </row>
+    <row r="11" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>338</v>
+      </c>
+      <c r="B11" s="43" t="s">
+        <v>337</v>
+      </c>
+      <c r="C11" s="26"/>
+      <c r="D11" s="27"/>
+      <c r="E11" s="26"/>
+      <c r="F11" s="27"/>
+      <c r="G11" s="26"/>
+      <c r="H11" s="27"/>
+      <c r="I11" s="26"/>
+      <c r="J11" s="27"/>
+      <c r="K11" s="26"/>
+      <c r="L11" s="27"/>
+      <c r="M11" s="26"/>
+      <c r="N11" s="27"/>
     </row>
     <row r="12" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A12" s="10" t="s">
+      <c r="A12" s="4" t="s">
+        <v>339</v>
+      </c>
+      <c r="B12" s="43" t="s">
+        <v>192</v>
+      </c>
+      <c r="C12" s="26"/>
+      <c r="D12" s="27"/>
+      <c r="E12" s="26"/>
+      <c r="F12" s="27"/>
+      <c r="G12" s="26"/>
+      <c r="H12" s="27"/>
+      <c r="I12" s="26"/>
+      <c r="J12" s="27"/>
+      <c r="K12" s="26"/>
+      <c r="L12" s="27"/>
+      <c r="M12" s="26"/>
+      <c r="N12" s="27"/>
+    </row>
+    <row r="14" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A14" s="10" t="s">
         <v>169</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B14" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="C14" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="D12" s="4" t="s">
+      <c r="D14" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="E12" s="4" t="s">
+      <c r="E14" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="F12" s="4" t="s">
+      <c r="F14" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="G12" s="4" t="s">
+      <c r="G14" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="H12" s="4" t="s">
+      <c r="H14" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="I12" s="4" t="s">
+      <c r="I14" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="J12" s="4" t="s">
+      <c r="J14" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="K12" s="4" t="s">
+      <c r="K14" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="L12" s="4" t="s">
+      <c r="L14" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="M12" s="4" t="s">
+      <c r="M14" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="N12" s="4" t="s">
+      <c r="N14" s="4" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="13" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A13" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="B13" s="14"/>
-      <c r="C13" s="18" t="s">
-        <v>170</v>
-      </c>
-      <c r="D13" s="19" t="s">
-        <v>171</v>
-      </c>
-      <c r="E13" s="20" t="s">
-        <v>172</v>
-      </c>
-      <c r="F13" s="21" t="s">
-        <v>173</v>
-      </c>
-      <c r="G13" s="22" t="s">
-        <v>174</v>
-      </c>
-      <c r="H13" s="23" t="s">
-        <v>175</v>
-      </c>
-      <c r="I13" s="24" t="s">
-        <v>176</v>
-      </c>
-      <c r="J13" s="18" t="s">
-        <v>177</v>
-      </c>
-      <c r="K13" s="19" t="s">
-        <v>178</v>
-      </c>
-      <c r="L13" s="20" t="s">
-        <v>179</v>
-      </c>
-      <c r="M13" s="21" t="s">
-        <v>180</v>
-      </c>
-      <c r="N13" s="22" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="14" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A14" s="15" t="s">
-        <v>53</v>
-      </c>
-      <c r="B14" s="25" t="s">
-        <v>11</v>
-      </c>
-      <c r="C14" s="28"/>
-      <c r="D14" s="29"/>
-      <c r="E14" s="28"/>
-      <c r="F14" s="29"/>
-      <c r="G14" s="28"/>
-      <c r="H14" s="29"/>
-      <c r="I14" s="28"/>
-      <c r="J14" s="29"/>
-      <c r="K14" s="28"/>
-      <c r="L14" s="29"/>
-      <c r="M14" s="28"/>
-      <c r="N14" s="29"/>
     </row>
     <row r="15" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A15" s="15" t="s">
-        <v>54</v>
-      </c>
-      <c r="B15" s="25" t="s">
-        <v>187</v>
-      </c>
-      <c r="C15" s="28"/>
-      <c r="D15" s="29"/>
-      <c r="E15" s="28"/>
-      <c r="F15" s="29"/>
-      <c r="G15" s="28"/>
-      <c r="H15" s="29"/>
-      <c r="I15" s="28"/>
-      <c r="J15" s="29"/>
-      <c r="K15" s="28"/>
-      <c r="L15" s="29"/>
-      <c r="M15" s="28"/>
-      <c r="N15" s="29"/>
+        <v>41</v>
+      </c>
+      <c r="B15" s="14"/>
+      <c r="C15" s="18" t="s">
+        <v>170</v>
+      </c>
+      <c r="D15" s="19" t="s">
+        <v>171</v>
+      </c>
+      <c r="E15" s="20" t="s">
+        <v>172</v>
+      </c>
+      <c r="F15" s="21" t="s">
+        <v>173</v>
+      </c>
+      <c r="G15" s="22" t="s">
+        <v>174</v>
+      </c>
+      <c r="H15" s="23" t="s">
+        <v>175</v>
+      </c>
+      <c r="I15" s="24" t="s">
+        <v>176</v>
+      </c>
+      <c r="J15" s="18" t="s">
+        <v>177</v>
+      </c>
+      <c r="K15" s="19" t="s">
+        <v>178</v>
+      </c>
+      <c r="L15" s="20" t="s">
+        <v>179</v>
+      </c>
+      <c r="M15" s="21" t="s">
+        <v>180</v>
+      </c>
+      <c r="N15" s="22" t="s">
+        <v>181</v>
+      </c>
     </row>
     <row r="16" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A16" s="15" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B16" s="25" t="s">
-        <v>188</v>
-      </c>
-      <c r="C16" s="28"/>
-      <c r="D16" s="29"/>
-      <c r="E16" s="28"/>
-      <c r="F16" s="29"/>
-      <c r="G16" s="28"/>
-      <c r="H16" s="29"/>
-      <c r="I16" s="28"/>
-      <c r="J16" s="29"/>
-      <c r="K16" s="28"/>
-      <c r="L16" s="29"/>
-      <c r="M16" s="28"/>
-      <c r="N16" s="29"/>
+        <v>11</v>
+      </c>
+      <c r="C16" s="26"/>
+      <c r="D16" s="27"/>
+      <c r="E16" s="26"/>
+      <c r="F16" s="27"/>
+      <c r="G16" s="26"/>
+      <c r="H16" s="27"/>
+      <c r="I16" s="26"/>
+      <c r="J16" s="27"/>
+      <c r="K16" s="26"/>
+      <c r="L16" s="27"/>
+      <c r="M16" s="26"/>
+      <c r="N16" s="27"/>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="15" t="s">
-        <v>56</v>
-      </c>
-      <c r="B17" s="17"/>
-      <c r="C17" s="30" t="s">
-        <v>189</v>
-      </c>
-      <c r="D17" s="30" t="s">
-        <v>189</v>
-      </c>
-      <c r="E17" s="30" t="s">
-        <v>189</v>
-      </c>
-      <c r="F17" s="30" t="s">
-        <v>189</v>
-      </c>
-      <c r="G17" s="30" t="s">
-        <v>189</v>
-      </c>
-      <c r="H17" s="30" t="s">
-        <v>189</v>
-      </c>
-      <c r="I17" s="30" t="s">
-        <v>189</v>
-      </c>
-      <c r="J17" s="30" t="s">
-        <v>189</v>
-      </c>
-      <c r="K17" s="30" t="s">
-        <v>189</v>
-      </c>
-      <c r="L17" s="30" t="s">
-        <v>189</v>
-      </c>
-      <c r="M17" s="30" t="s">
-        <v>189</v>
-      </c>
-      <c r="N17" s="30" t="s">
-        <v>189</v>
-      </c>
+        <v>54</v>
+      </c>
+      <c r="B17" s="25" t="s">
+        <v>187</v>
+      </c>
+      <c r="C17" s="26"/>
+      <c r="D17" s="27"/>
+      <c r="E17" s="26"/>
+      <c r="F17" s="27"/>
+      <c r="G17" s="26"/>
+      <c r="H17" s="27"/>
+      <c r="I17" s="26"/>
+      <c r="J17" s="27"/>
+      <c r="K17" s="26"/>
+      <c r="L17" s="27"/>
+      <c r="M17" s="26"/>
+      <c r="N17" s="27"/>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" s="15" t="s">
-        <v>57</v>
-      </c>
-      <c r="B18" s="38" t="s">
-        <v>190</v>
-      </c>
-      <c r="C18" s="28"/>
-      <c r="D18" s="29"/>
-      <c r="E18" s="28"/>
-      <c r="F18" s="29"/>
-      <c r="G18" s="28"/>
-      <c r="H18" s="29"/>
-      <c r="I18" s="28"/>
-      <c r="J18" s="29"/>
-      <c r="K18" s="28"/>
-      <c r="L18" s="29"/>
-      <c r="M18" s="28"/>
-      <c r="N18" s="29"/>
+        <v>55</v>
+      </c>
+      <c r="B18" s="25" t="s">
+        <v>188</v>
+      </c>
+      <c r="C18" s="26"/>
+      <c r="D18" s="27"/>
+      <c r="E18" s="26"/>
+      <c r="F18" s="27"/>
+      <c r="G18" s="26"/>
+      <c r="H18" s="27"/>
+      <c r="I18" s="26"/>
+      <c r="J18" s="27"/>
+      <c r="K18" s="26"/>
+      <c r="L18" s="27"/>
+      <c r="M18" s="26"/>
+      <c r="N18" s="27"/>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" s="15" t="s">
-        <v>58</v>
-      </c>
-      <c r="B19" s="27" t="s">
-        <v>191</v>
-      </c>
-      <c r="C19" s="28"/>
-      <c r="D19" s="29"/>
-      <c r="E19" s="28"/>
-      <c r="F19" s="29"/>
-      <c r="G19" s="28"/>
-      <c r="H19" s="29"/>
-      <c r="I19" s="28"/>
-      <c r="J19" s="29"/>
-      <c r="K19" s="28"/>
-      <c r="L19" s="29"/>
-      <c r="M19" s="28"/>
-      <c r="N19" s="29"/>
+        <v>56</v>
+      </c>
+      <c r="B19" s="17"/>
+      <c r="C19" s="28" t="s">
+        <v>189</v>
+      </c>
+      <c r="D19" s="28" t="s">
+        <v>189</v>
+      </c>
+      <c r="E19" s="28" t="s">
+        <v>189</v>
+      </c>
+      <c r="F19" s="28" t="s">
+        <v>189</v>
+      </c>
+      <c r="G19" s="28" t="s">
+        <v>189</v>
+      </c>
+      <c r="H19" s="28" t="s">
+        <v>189</v>
+      </c>
+      <c r="I19" s="28" t="s">
+        <v>189</v>
+      </c>
+      <c r="J19" s="28" t="s">
+        <v>189</v>
+      </c>
+      <c r="K19" s="28" t="s">
+        <v>189</v>
+      </c>
+      <c r="L19" s="28" t="s">
+        <v>189</v>
+      </c>
+      <c r="M19" s="28" t="s">
+        <v>189</v>
+      </c>
+      <c r="N19" s="28" t="s">
+        <v>189</v>
+      </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="B20" s="42" t="s">
+        <v>190</v>
+      </c>
+      <c r="C20" s="26"/>
+      <c r="D20" s="27"/>
+      <c r="E20" s="26"/>
+      <c r="F20" s="27"/>
+      <c r="G20" s="26"/>
+      <c r="H20" s="27"/>
+      <c r="I20" s="26"/>
+      <c r="J20" s="27"/>
+      <c r="K20" s="26"/>
+      <c r="L20" s="27"/>
+      <c r="M20" s="26"/>
+      <c r="N20" s="27"/>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A21" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="B21" s="42" t="s">
+        <v>365</v>
+      </c>
+      <c r="C21" s="26"/>
+      <c r="D21" s="27"/>
+      <c r="E21" s="26"/>
+      <c r="F21" s="27"/>
+      <c r="G21" s="26"/>
+      <c r="H21" s="27"/>
+      <c r="I21" s="26"/>
+      <c r="J21" s="27"/>
+      <c r="K21" s="26"/>
+      <c r="L21" s="27"/>
+      <c r="M21" s="26"/>
+      <c r="N21" s="27"/>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A22" s="15" t="s">
         <v>59</v>
       </c>
-      <c r="B20" s="27" t="s">
+      <c r="B22" s="42" t="s">
+        <v>366</v>
+      </c>
+      <c r="C22" s="26"/>
+      <c r="D22" s="27"/>
+      <c r="E22" s="26"/>
+      <c r="F22" s="27"/>
+      <c r="G22" s="26"/>
+      <c r="H22" s="27"/>
+      <c r="I22" s="26"/>
+      <c r="J22" s="27"/>
+      <c r="K22" s="26"/>
+      <c r="L22" s="27"/>
+      <c r="M22" s="26"/>
+      <c r="N22" s="27"/>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A23" s="15" t="s">
+        <v>159</v>
+      </c>
+      <c r="B23" s="43" t="s">
+        <v>369</v>
+      </c>
+      <c r="C23" s="26"/>
+      <c r="D23" s="27"/>
+      <c r="E23" s="26"/>
+      <c r="F23" s="27"/>
+      <c r="G23" s="26"/>
+      <c r="H23" s="27"/>
+      <c r="I23" s="26"/>
+      <c r="J23" s="27"/>
+      <c r="K23" s="26"/>
+      <c r="L23" s="27"/>
+      <c r="M23" s="26"/>
+      <c r="N23" s="27"/>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A24" s="4" t="s">
+        <v>338</v>
+      </c>
+      <c r="B24" s="43" t="s">
+        <v>370</v>
+      </c>
+      <c r="C24" s="26"/>
+      <c r="D24" s="27"/>
+      <c r="E24" s="26"/>
+      <c r="F24" s="27"/>
+      <c r="G24" s="26"/>
+      <c r="H24" s="27"/>
+      <c r="I24" s="26"/>
+      <c r="J24" s="27"/>
+      <c r="K24" s="26"/>
+      <c r="L24" s="27"/>
+      <c r="M24" s="26"/>
+      <c r="N24" s="27"/>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A25" s="4" t="s">
+        <v>339</v>
+      </c>
+      <c r="B25" s="43" t="s">
         <v>192</v>
       </c>
-      <c r="C20" s="28"/>
-      <c r="D20" s="29"/>
-      <c r="E20" s="28"/>
-      <c r="F20" s="29"/>
-      <c r="G20" s="28"/>
-      <c r="H20" s="29"/>
-      <c r="I20" s="28"/>
-      <c r="J20" s="29"/>
-      <c r="K20" s="28"/>
-      <c r="L20" s="29"/>
-      <c r="M20" s="28"/>
-      <c r="N20" s="29"/>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A21" s="4" t="s">
-        <v>159</v>
-      </c>
-      <c r="B21" s="27" t="s">
-        <v>193</v>
-      </c>
-      <c r="C21" s="28"/>
-      <c r="D21" s="29"/>
-      <c r="E21" s="28"/>
-      <c r="F21" s="29"/>
-      <c r="G21" s="28"/>
-      <c r="H21" s="29"/>
-      <c r="I21" s="28"/>
-      <c r="J21" s="29"/>
-      <c r="K21" s="28"/>
-      <c r="L21" s="29"/>
-      <c r="M21" s="28"/>
-      <c r="N21" s="29"/>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A23" s="10" t="s">
+      <c r="C25" s="26"/>
+      <c r="D25" s="27"/>
+      <c r="E25" s="26"/>
+      <c r="F25" s="27"/>
+      <c r="G25" s="26"/>
+      <c r="H25" s="27"/>
+      <c r="I25" s="26"/>
+      <c r="J25" s="27"/>
+      <c r="K25" s="26"/>
+      <c r="L25" s="27"/>
+      <c r="M25" s="26"/>
+      <c r="N25" s="27"/>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A27" s="10" t="s">
         <v>169</v>
       </c>
-      <c r="B23" s="4" t="s">
+      <c r="B27" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="C23" s="4" t="s">
+      <c r="C27" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="D23" s="4" t="s">
+      <c r="D27" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="E23" s="4" t="s">
+      <c r="E27" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="F23" s="4" t="s">
+      <c r="F27" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="G23" s="4" t="s">
+      <c r="G27" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="H23" s="4" t="s">
+      <c r="H27" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="I23" s="4" t="s">
+      <c r="I27" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="J23" s="4" t="s">
+      <c r="J27" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="K23" s="4" t="s">
+      <c r="K27" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="L23" s="4" t="s">
+      <c r="L27" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="M23" s="4" t="s">
+      <c r="M27" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="N23" s="4" t="s">
+      <c r="N27" s="4" t="s">
         <v>121</v>
-      </c>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A24" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="B24" s="14"/>
-      <c r="C24" s="18" t="s">
-        <v>194</v>
-      </c>
-      <c r="D24" s="19" t="s">
-        <v>195</v>
-      </c>
-      <c r="E24" s="20" t="s">
-        <v>196</v>
-      </c>
-      <c r="F24" s="21" t="s">
-        <v>197</v>
-      </c>
-      <c r="G24" s="22" t="s">
-        <v>198</v>
-      </c>
-      <c r="H24" s="23" t="s">
-        <v>199</v>
-      </c>
-      <c r="I24" s="24" t="s">
-        <v>200</v>
-      </c>
-      <c r="J24" s="18" t="s">
-        <v>201</v>
-      </c>
-      <c r="K24" s="19" t="s">
-        <v>202</v>
-      </c>
-      <c r="L24" s="20" t="s">
-        <v>203</v>
-      </c>
-      <c r="M24" s="21" t="s">
-        <v>204</v>
-      </c>
-      <c r="N24" s="22" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A25" s="15" t="s">
-        <v>53</v>
-      </c>
-      <c r="B25" s="25" t="s">
-        <v>206</v>
-      </c>
-      <c r="C25" s="28" t="s">
-        <v>207</v>
-      </c>
-      <c r="D25" s="29" t="s">
-        <v>208</v>
-      </c>
-      <c r="E25" s="28" t="s">
-        <v>209</v>
-      </c>
-      <c r="F25" s="29" t="s">
-        <v>210</v>
-      </c>
-      <c r="G25" s="28" t="s">
-        <v>211</v>
-      </c>
-      <c r="H25" s="29" t="s">
-        <v>212</v>
-      </c>
-      <c r="I25" s="28" t="s">
-        <v>213</v>
-      </c>
-      <c r="J25" s="29" t="s">
-        <v>214</v>
-      </c>
-      <c r="K25" s="28" t="s">
-        <v>215</v>
-      </c>
-      <c r="L25" s="29" t="s">
-        <v>216</v>
-      </c>
-      <c r="M25" s="28" t="s">
-        <v>217</v>
-      </c>
-      <c r="N25" s="29" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A26" s="15" t="s">
-        <v>54</v>
-      </c>
-      <c r="B26" s="25" t="s">
-        <v>219</v>
-      </c>
-      <c r="C26" s="28" t="s">
-        <v>220</v>
-      </c>
-      <c r="D26" s="29" t="s">
-        <v>221</v>
-      </c>
-      <c r="E26" s="28" t="s">
-        <v>222</v>
-      </c>
-      <c r="F26" s="29" t="s">
-        <v>223</v>
-      </c>
-      <c r="G26" s="28" t="s">
-        <v>224</v>
-      </c>
-      <c r="H26" s="29" t="s">
-        <v>225</v>
-      </c>
-      <c r="I26" s="28" t="s">
-        <v>226</v>
-      </c>
-      <c r="J26" s="29" t="s">
-        <v>227</v>
-      </c>
-      <c r="K26" s="28" t="s">
-        <v>228</v>
-      </c>
-      <c r="L26" s="29" t="s">
-        <v>229</v>
-      </c>
-      <c r="M26" s="28" t="s">
-        <v>230</v>
-      </c>
-      <c r="N26" s="29" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A27" s="15" t="s">
-        <v>55</v>
-      </c>
-      <c r="B27" s="25" t="s">
-        <v>232</v>
-      </c>
-      <c r="C27" s="28" t="s">
-        <v>233</v>
-      </c>
-      <c r="D27" s="29" t="s">
-        <v>234</v>
-      </c>
-      <c r="E27" s="28" t="s">
-        <v>235</v>
-      </c>
-      <c r="F27" s="29" t="s">
-        <v>236</v>
-      </c>
-      <c r="G27" s="28" t="s">
-        <v>237</v>
-      </c>
-      <c r="H27" s="29" t="s">
-        <v>238</v>
-      </c>
-      <c r="I27" s="28" t="s">
-        <v>239</v>
-      </c>
-      <c r="J27" s="29" t="s">
-        <v>240</v>
-      </c>
-      <c r="K27" s="28" t="s">
-        <v>241</v>
-      </c>
-      <c r="L27" s="29" t="s">
-        <v>242</v>
-      </c>
-      <c r="M27" s="28" t="s">
-        <v>243</v>
-      </c>
-      <c r="N27" s="29" t="s">
-        <v>244</v>
       </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" s="15" t="s">
-        <v>56</v>
-      </c>
-      <c r="B28" s="17"/>
-      <c r="C28" s="30" t="s">
-        <v>310</v>
-      </c>
-      <c r="D28" s="30" t="s">
-        <v>311</v>
-      </c>
-      <c r="E28" s="30" t="s">
-        <v>312</v>
-      </c>
-      <c r="F28" s="30" t="s">
-        <v>313</v>
-      </c>
-      <c r="G28" s="30" t="s">
-        <v>314</v>
-      </c>
-      <c r="H28" s="30" t="s">
-        <v>315</v>
-      </c>
-      <c r="I28" s="30" t="s">
-        <v>316</v>
-      </c>
-      <c r="J28" s="30" t="s">
-        <v>317</v>
-      </c>
-      <c r="K28" s="30" t="s">
-        <v>318</v>
-      </c>
-      <c r="L28" s="30" t="s">
-        <v>319</v>
-      </c>
-      <c r="M28" s="30" t="s">
-        <v>320</v>
-      </c>
-      <c r="N28" s="30" t="s">
-        <v>321</v>
+        <v>41</v>
+      </c>
+      <c r="B28" s="14"/>
+      <c r="C28" s="18" t="s">
+        <v>193</v>
+      </c>
+      <c r="D28" s="19" t="s">
+        <v>194</v>
+      </c>
+      <c r="E28" s="20" t="s">
+        <v>195</v>
+      </c>
+      <c r="F28" s="21" t="s">
+        <v>196</v>
+      </c>
+      <c r="G28" s="22" t="s">
+        <v>197</v>
+      </c>
+      <c r="H28" s="23" t="s">
+        <v>198</v>
+      </c>
+      <c r="I28" s="24" t="s">
+        <v>199</v>
+      </c>
+      <c r="J28" s="18" t="s">
+        <v>200</v>
+      </c>
+      <c r="K28" s="19" t="s">
+        <v>201</v>
+      </c>
+      <c r="L28" s="20" t="s">
+        <v>202</v>
+      </c>
+      <c r="M28" s="21" t="s">
+        <v>203</v>
+      </c>
+      <c r="N28" s="22" t="s">
+        <v>204</v>
       </c>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" s="15" t="s">
-        <v>57</v>
-      </c>
-      <c r="B29" s="27" t="s">
-        <v>245</v>
-      </c>
-      <c r="C29" s="28" t="s">
-        <v>246</v>
-      </c>
-      <c r="D29" s="29" t="s">
-        <v>247</v>
-      </c>
-      <c r="E29" s="28" t="s">
-        <v>248</v>
-      </c>
-      <c r="F29" s="29" t="s">
-        <v>249</v>
-      </c>
-      <c r="G29" s="28" t="s">
-        <v>250</v>
-      </c>
-      <c r="H29" s="29" t="s">
-        <v>251</v>
-      </c>
-      <c r="I29" s="28" t="s">
-        <v>252</v>
-      </c>
-      <c r="J29" s="29" t="s">
-        <v>253</v>
-      </c>
-      <c r="K29" s="28" t="s">
-        <v>254</v>
-      </c>
-      <c r="L29" s="29" t="s">
-        <v>255</v>
-      </c>
-      <c r="M29" s="28" t="s">
-        <v>256</v>
-      </c>
-      <c r="N29" s="29" t="s">
-        <v>257</v>
+        <v>53</v>
+      </c>
+      <c r="B29" s="25" t="s">
+        <v>205</v>
+      </c>
+      <c r="C29" s="26" t="s">
+        <v>206</v>
+      </c>
+      <c r="D29" s="27" t="s">
+        <v>207</v>
+      </c>
+      <c r="E29" s="26" t="s">
+        <v>208</v>
+      </c>
+      <c r="F29" s="27" t="s">
+        <v>209</v>
+      </c>
+      <c r="G29" s="26" t="s">
+        <v>210</v>
+      </c>
+      <c r="H29" s="27" t="s">
+        <v>211</v>
+      </c>
+      <c r="I29" s="26" t="s">
+        <v>212</v>
+      </c>
+      <c r="J29" s="27" t="s">
+        <v>213</v>
+      </c>
+      <c r="K29" s="26" t="s">
+        <v>214</v>
+      </c>
+      <c r="L29" s="27" t="s">
+        <v>215</v>
+      </c>
+      <c r="M29" s="26" t="s">
+        <v>216</v>
+      </c>
+      <c r="N29" s="27" t="s">
+        <v>217</v>
       </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" s="15" t="s">
-        <v>58</v>
-      </c>
-      <c r="B30" s="27" t="s">
-        <v>258</v>
-      </c>
-      <c r="C30" s="28" t="s">
-        <v>259</v>
-      </c>
-      <c r="D30" s="29" t="s">
-        <v>260</v>
-      </c>
-      <c r="E30" s="28" t="s">
-        <v>261</v>
-      </c>
-      <c r="F30" s="29" t="s">
-        <v>262</v>
-      </c>
-      <c r="G30" s="28" t="s">
-        <v>263</v>
-      </c>
-      <c r="H30" s="29" t="s">
-        <v>264</v>
-      </c>
-      <c r="I30" s="28" t="s">
-        <v>265</v>
-      </c>
-      <c r="J30" s="29" t="s">
-        <v>266</v>
-      </c>
-      <c r="K30" s="28" t="s">
-        <v>267</v>
-      </c>
-      <c r="L30" s="29" t="s">
-        <v>268</v>
-      </c>
-      <c r="M30" s="28" t="s">
-        <v>269</v>
-      </c>
-      <c r="N30" s="29" t="s">
-        <v>270</v>
+        <v>54</v>
+      </c>
+      <c r="B30" s="25" t="s">
+        <v>218</v>
+      </c>
+      <c r="C30" s="26" t="s">
+        <v>219</v>
+      </c>
+      <c r="D30" s="27" t="s">
+        <v>220</v>
+      </c>
+      <c r="E30" s="26" t="s">
+        <v>221</v>
+      </c>
+      <c r="F30" s="27" t="s">
+        <v>222</v>
+      </c>
+      <c r="G30" s="26" t="s">
+        <v>223</v>
+      </c>
+      <c r="H30" s="27" t="s">
+        <v>224</v>
+      </c>
+      <c r="I30" s="26" t="s">
+        <v>225</v>
+      </c>
+      <c r="J30" s="27" t="s">
+        <v>226</v>
+      </c>
+      <c r="K30" s="26" t="s">
+        <v>227</v>
+      </c>
+      <c r="L30" s="27" t="s">
+        <v>228</v>
+      </c>
+      <c r="M30" s="26" t="s">
+        <v>229</v>
+      </c>
+      <c r="N30" s="27" t="s">
+        <v>230</v>
       </c>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" s="15" t="s">
-        <v>59</v>
-      </c>
-      <c r="B31" s="27" t="s">
-        <v>271</v>
-      </c>
-      <c r="C31" s="28" t="s">
-        <v>272</v>
-      </c>
-      <c r="D31" s="29" t="s">
-        <v>273</v>
-      </c>
-      <c r="E31" s="28" t="s">
-        <v>274</v>
-      </c>
-      <c r="F31" s="29" t="s">
-        <v>275</v>
-      </c>
-      <c r="G31" s="28" t="s">
-        <v>276</v>
-      </c>
-      <c r="H31" s="29" t="s">
-        <v>277</v>
-      </c>
-      <c r="I31" s="28" t="s">
-        <v>278</v>
-      </c>
-      <c r="J31" s="29" t="s">
-        <v>279</v>
-      </c>
-      <c r="K31" s="28" t="s">
-        <v>280</v>
-      </c>
-      <c r="L31" s="29" t="s">
-        <v>281</v>
-      </c>
-      <c r="M31" s="28" t="s">
-        <v>282</v>
-      </c>
-      <c r="N31" s="29" t="s">
-        <v>283</v>
+        <v>55</v>
+      </c>
+      <c r="B31" s="25" t="s">
+        <v>231</v>
+      </c>
+      <c r="C31" s="26" t="s">
+        <v>232</v>
+      </c>
+      <c r="D31" s="27" t="s">
+        <v>233</v>
+      </c>
+      <c r="E31" s="26" t="s">
+        <v>234</v>
+      </c>
+      <c r="F31" s="27" t="s">
+        <v>235</v>
+      </c>
+      <c r="G31" s="26" t="s">
+        <v>236</v>
+      </c>
+      <c r="H31" s="27" t="s">
+        <v>237</v>
+      </c>
+      <c r="I31" s="26" t="s">
+        <v>238</v>
+      </c>
+      <c r="J31" s="27" t="s">
+        <v>239</v>
+      </c>
+      <c r="K31" s="26" t="s">
+        <v>240</v>
+      </c>
+      <c r="L31" s="27" t="s">
+        <v>241</v>
+      </c>
+      <c r="M31" s="26" t="s">
+        <v>242</v>
+      </c>
+      <c r="N31" s="27" t="s">
+        <v>243</v>
       </c>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="B32" s="17"/>
+      <c r="C32" s="28" t="s">
+        <v>309</v>
+      </c>
+      <c r="D32" s="28" t="s">
+        <v>310</v>
+      </c>
+      <c r="E32" s="28" t="s">
+        <v>311</v>
+      </c>
+      <c r="F32" s="28" t="s">
+        <v>312</v>
+      </c>
+      <c r="G32" s="28" t="s">
+        <v>313</v>
+      </c>
+      <c r="H32" s="28" t="s">
+        <v>314</v>
+      </c>
+      <c r="I32" s="28" t="s">
+        <v>315</v>
+      </c>
+      <c r="J32" s="28" t="s">
+        <v>316</v>
+      </c>
+      <c r="K32" s="28" t="s">
+        <v>317</v>
+      </c>
+      <c r="L32" s="28" t="s">
+        <v>318</v>
+      </c>
+      <c r="M32" s="28" t="s">
+        <v>319</v>
+      </c>
+      <c r="N32" s="28" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A33" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="B33" s="42" t="s">
+        <v>244</v>
+      </c>
+      <c r="C33" s="26" t="s">
+        <v>245</v>
+      </c>
+      <c r="D33" s="27" t="s">
+        <v>246</v>
+      </c>
+      <c r="E33" s="26" t="s">
+        <v>247</v>
+      </c>
+      <c r="F33" s="27" t="s">
+        <v>248</v>
+      </c>
+      <c r="G33" s="26" t="s">
+        <v>249</v>
+      </c>
+      <c r="H33" s="27" t="s">
+        <v>250</v>
+      </c>
+      <c r="I33" s="26" t="s">
+        <v>251</v>
+      </c>
+      <c r="J33" s="27" t="s">
+        <v>252</v>
+      </c>
+      <c r="K33" s="26" t="s">
+        <v>253</v>
+      </c>
+      <c r="L33" s="27" t="s">
+        <v>254</v>
+      </c>
+      <c r="M33" s="26" t="s">
+        <v>255</v>
+      </c>
+      <c r="N33" s="27" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A34" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="B34" s="42" t="s">
+        <v>257</v>
+      </c>
+      <c r="C34" s="26" t="s">
+        <v>258</v>
+      </c>
+      <c r="D34" s="27" t="s">
+        <v>259</v>
+      </c>
+      <c r="E34" s="26" t="s">
+        <v>260</v>
+      </c>
+      <c r="F34" s="27" t="s">
+        <v>261</v>
+      </c>
+      <c r="G34" s="26" t="s">
+        <v>262</v>
+      </c>
+      <c r="H34" s="27" t="s">
+        <v>263</v>
+      </c>
+      <c r="I34" s="26" t="s">
+        <v>264</v>
+      </c>
+      <c r="J34" s="27" t="s">
+        <v>265</v>
+      </c>
+      <c r="K34" s="26" t="s">
+        <v>266</v>
+      </c>
+      <c r="L34" s="27" t="s">
+        <v>267</v>
+      </c>
+      <c r="M34" s="26" t="s">
+        <v>268</v>
+      </c>
+      <c r="N34" s="27" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A35" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="B35" s="42" t="s">
+        <v>270</v>
+      </c>
+      <c r="C35" s="26" t="s">
+        <v>271</v>
+      </c>
+      <c r="D35" s="27" t="s">
+        <v>272</v>
+      </c>
+      <c r="E35" s="26" t="s">
+        <v>273</v>
+      </c>
+      <c r="F35" s="27" t="s">
+        <v>274</v>
+      </c>
+      <c r="G35" s="26" t="s">
+        <v>275</v>
+      </c>
+      <c r="H35" s="27" t="s">
+        <v>276</v>
+      </c>
+      <c r="I35" s="26" t="s">
+        <v>277</v>
+      </c>
+      <c r="J35" s="27" t="s">
+        <v>278</v>
+      </c>
+      <c r="K35" s="26" t="s">
+        <v>279</v>
+      </c>
+      <c r="L35" s="27" t="s">
+        <v>280</v>
+      </c>
+      <c r="M35" s="26" t="s">
+        <v>281</v>
+      </c>
+      <c r="N35" s="27" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A36" s="15" t="s">
         <v>159</v>
       </c>
-      <c r="B32" s="27" t="s">
+      <c r="B36" s="43" t="s">
+        <v>283</v>
+      </c>
+      <c r="C36" s="26" t="s">
         <v>284</v>
       </c>
-      <c r="C32" s="28" t="s">
+      <c r="D36" s="27" t="s">
         <v>285</v>
       </c>
-      <c r="D32" s="29" t="s">
+      <c r="E36" s="26" t="s">
         <v>286</v>
       </c>
-      <c r="E32" s="28" t="s">
+      <c r="F36" s="27" t="s">
         <v>287</v>
       </c>
-      <c r="F32" s="29" t="s">
+      <c r="G36" s="26" t="s">
         <v>288</v>
       </c>
-      <c r="G32" s="28" t="s">
+      <c r="H36" s="27" t="s">
         <v>289</v>
       </c>
-      <c r="H32" s="29" t="s">
+      <c r="I36" s="26" t="s">
         <v>290</v>
       </c>
-      <c r="I32" s="28" t="s">
+      <c r="J36" s="27" t="s">
         <v>291</v>
       </c>
-      <c r="J32" s="29" t="s">
+      <c r="K36" s="26" t="s">
         <v>292</v>
       </c>
-      <c r="K32" s="28" t="s">
+      <c r="L36" s="27" t="s">
         <v>293</v>
       </c>
-      <c r="L32" s="29" t="s">
+      <c r="M36" s="26" t="s">
         <v>294</v>
       </c>
-      <c r="M32" s="28" t="s">
+      <c r="N36" s="27" t="s">
         <v>295</v>
       </c>
-      <c r="N32" s="29" t="s">
-        <v>296</v>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A37" s="4" t="s">
+        <v>338</v>
+      </c>
+      <c r="B37" s="43" t="s">
+        <v>323</v>
+      </c>
+      <c r="C37" s="26" t="s">
+        <v>340</v>
+      </c>
+      <c r="D37" s="27" t="s">
+        <v>341</v>
+      </c>
+      <c r="E37" s="26" t="s">
+        <v>342</v>
+      </c>
+      <c r="F37" s="27" t="s">
+        <v>343</v>
+      </c>
+      <c r="G37" s="26" t="s">
+        <v>344</v>
+      </c>
+      <c r="H37" s="27" t="s">
+        <v>345</v>
+      </c>
+      <c r="I37" s="26" t="s">
+        <v>346</v>
+      </c>
+      <c r="J37" s="27" t="s">
+        <v>347</v>
+      </c>
+      <c r="K37" s="26" t="s">
+        <v>348</v>
+      </c>
+      <c r="L37" s="27" t="s">
+        <v>349</v>
+      </c>
+      <c r="M37" s="26" t="s">
+        <v>350</v>
+      </c>
+      <c r="N37" s="27" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A38" s="4" t="s">
+        <v>339</v>
+      </c>
+      <c r="B38" s="43" t="s">
+        <v>352</v>
+      </c>
+      <c r="C38" s="26" t="s">
+        <v>353</v>
+      </c>
+      <c r="D38" s="27" t="s">
+        <v>354</v>
+      </c>
+      <c r="E38" s="26" t="s">
+        <v>355</v>
+      </c>
+      <c r="F38" s="27" t="s">
+        <v>356</v>
+      </c>
+      <c r="G38" s="26" t="s">
+        <v>357</v>
+      </c>
+      <c r="H38" s="27" t="s">
+        <v>358</v>
+      </c>
+      <c r="I38" s="26" t="s">
+        <v>359</v>
+      </c>
+      <c r="J38" s="27" t="s">
+        <v>360</v>
+      </c>
+      <c r="K38" s="26" t="s">
+        <v>361</v>
+      </c>
+      <c r="L38" s="27" t="s">
+        <v>362</v>
+      </c>
+      <c r="M38" s="26" t="s">
+        <v>363</v>
+      </c>
+      <c r="N38" s="27" t="s">
+        <v>364</v>
       </c>
     </row>
   </sheetData>
@@ -4587,8 +4858,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47B91243-A115-4684-A5E9-C7F45B75B539}">
   <dimension ref="A1:L22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L22" sqref="L22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N20" sqref="N20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4599,7 +4870,7 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>42</v>
@@ -4624,34 +4895,34 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="44" t="s">
         <v>41</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="C2" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="39" t="s">
+      <c r="D2" s="36" t="s">
+        <v>326</v>
+      </c>
+      <c r="E2" s="19" t="s">
+        <v>332</v>
+      </c>
+      <c r="F2" s="37" t="s">
+        <v>324</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>325</v>
+      </c>
+      <c r="H2" s="14" t="s">
         <v>327</v>
-      </c>
-      <c r="E2" s="19" t="s">
-        <v>333</v>
-      </c>
-      <c r="F2" s="40" t="s">
-        <v>325</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>326</v>
-      </c>
-      <c r="H2" s="14" t="s">
-        <v>328</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>42</v>
@@ -4676,29 +4947,29 @@
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="9" t="s">
+      <c r="A6" s="44" t="s">
         <v>41</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>324</v>
+        <v>367</v>
       </c>
       <c r="C6" s="3" t="s">
+        <v>328</v>
+      </c>
+      <c r="D6" s="3" t="s">
         <v>329</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="E6" s="3" t="s">
         <v>330</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="F6" s="3" t="s">
         <v>331</v>
       </c>
-      <c r="F6" s="3" t="s">
-        <v>332</v>
-      </c>
       <c r="G6" s="3" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>335</v>
+        <v>368</v>
       </c>
     </row>
     <row r="22" spans="12:12" x14ac:dyDescent="0.25">
@@ -4714,19 +4985,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE7D2FF7-64A1-41EF-8B15-47A7AFD3DE78}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L25" sqref="L25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.5703125" customWidth="1"/>
-    <col min="2" max="2" width="40.7109375" style="44" customWidth="1"/>
+    <col min="2" max="2" width="40.7109375" style="38" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>42</v>
@@ -4737,12 +5008,12 @@
         <v>41</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>42</v>
@@ -4753,7 +5024,7 @@
         <v>41</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Se crea root support
</commit_message>
<xml_diff>
--- a/distribucion.xlsx
+++ b/distribucion.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27932"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Registro_defectos_SEHO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D501BC49-F73E-442D-A8F6-EC105866AA91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E1B7020-DFF9-4C00-BD25-AEEA8ED4C917}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="5" xr2:uid="{C5A581BF-84BA-4755-84C9-6391AAA71289}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="8" xr2:uid="{C5A581BF-84BA-4755-84C9-6391AAA71289}"/>
   </bookViews>
   <sheets>
     <sheet name="Frame0" sheetId="2" r:id="rId1"/>
@@ -20,6 +20,8 @@
     <sheet name="Frame4" sheetId="6" r:id="rId5"/>
     <sheet name="Frame5" sheetId="7" r:id="rId6"/>
     <sheet name="root_defect" sheetId="8" r:id="rId7"/>
+    <sheet name="frame0_rs" sheetId="9" r:id="rId8"/>
+    <sheet name="frame1_rs" sheetId="10" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,6 +38,9 @@
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
         <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
+    </ext>
+    <ext xmlns:xlwcv="http://schemas.microsoft.com/office/spreadsheetml/2024/workbookCompatibilityVersion" uri="{D14903EA-33C4-47F7-8F05-3474C54BE107}">
+      <xlwcv:version setVersion="1"/>
     </ext>
   </extLst>
 </workbook>
@@ -74,7 +79,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="589" uniqueCount="371">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="617" uniqueCount="383">
   <si>
     <t>FA08</t>
   </si>
@@ -1187,13 +1192,49 @@
   </si>
   <si>
     <t>Cant.Defect:</t>
+  </si>
+  <si>
+    <t>frame0_rs</t>
+  </si>
+  <si>
+    <t>Soporte</t>
+  </si>
+  <si>
+    <t>label_rs_0</t>
+  </si>
+  <si>
+    <t>Ingeniería</t>
+  </si>
+  <si>
+    <t>Calidad</t>
+  </si>
+  <si>
+    <t>Producción</t>
+  </si>
+  <si>
+    <t>Todos</t>
+  </si>
+  <si>
+    <t>frame1_rs</t>
+  </si>
+  <si>
+    <t>button_rs_0</t>
+  </si>
+  <si>
+    <t>button_rs_1</t>
+  </si>
+  <si>
+    <t>button_rs_2</t>
+  </si>
+  <si>
+    <t>button_rs_3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1254,8 +1295,24 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="22">
+  <fills count="23">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1382,6 +1439,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="8">
     <border>
@@ -1480,7 +1543,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1588,6 +1651,30 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1596,15 +1683,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="21" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2770,18 +2848,18 @@
       <c r="A2" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="B2" s="40" t="s">
+      <c r="B2" s="48" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="40"/>
-      <c r="D2" s="40"/>
-      <c r="E2" s="40"/>
-      <c r="F2" s="40"/>
-      <c r="G2" s="40"/>
-      <c r="H2" s="40"/>
-      <c r="I2" s="40"/>
-      <c r="J2" s="40"/>
-      <c r="K2" s="40"/>
+      <c r="C2" s="48"/>
+      <c r="D2" s="48"/>
+      <c r="E2" s="48"/>
+      <c r="F2" s="48"/>
+      <c r="G2" s="48"/>
+      <c r="H2" s="48"/>
+      <c r="I2" s="48"/>
+      <c r="J2" s="48"/>
+      <c r="K2" s="48"/>
     </row>
     <row r="3" spans="1:11" ht="24" x14ac:dyDescent="0.4">
       <c r="A3" s="9" t="s">
@@ -2940,12 +3018,12 @@
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
-      <c r="E9" s="41" t="s">
+      <c r="E9" s="49" t="s">
         <v>10</v>
       </c>
-      <c r="F9" s="41"/>
-      <c r="G9" s="41"/>
-      <c r="H9" s="41"/>
+      <c r="F9" s="49"/>
+      <c r="G9" s="49"/>
+      <c r="H9" s="49"/>
       <c r="I9" s="1"/>
       <c r="J9" s="2"/>
       <c r="K9" s="2"/>
@@ -2957,10 +3035,10 @@
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
-      <c r="E10" s="39"/>
-      <c r="F10" s="39"/>
-      <c r="G10" s="39"/>
-      <c r="H10" s="39"/>
+      <c r="E10" s="47"/>
+      <c r="F10" s="47"/>
+      <c r="G10" s="47"/>
+      <c r="H10" s="47"/>
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
       <c r="K10" s="1"/>
@@ -3004,18 +3082,18 @@
       <c r="A14" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="B14" s="40" t="s">
+      <c r="B14" s="48" t="s">
         <v>60</v>
       </c>
-      <c r="C14" s="40"/>
-      <c r="D14" s="40"/>
-      <c r="E14" s="40"/>
-      <c r="F14" s="40"/>
-      <c r="G14" s="40"/>
-      <c r="H14" s="40"/>
-      <c r="I14" s="40"/>
-      <c r="J14" s="40"/>
-      <c r="K14" s="40"/>
+      <c r="C14" s="48"/>
+      <c r="D14" s="48"/>
+      <c r="E14" s="48"/>
+      <c r="F14" s="48"/>
+      <c r="G14" s="48"/>
+      <c r="H14" s="48"/>
+      <c r="I14" s="48"/>
+      <c r="J14" s="48"/>
+      <c r="K14" s="48"/>
     </row>
     <row r="15" spans="1:11" ht="24" x14ac:dyDescent="0.4">
       <c r="A15" s="9" t="s">
@@ -3234,12 +3312,12 @@
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
-      <c r="E21" s="41" t="s">
+      <c r="E21" s="49" t="s">
         <v>130</v>
       </c>
-      <c r="F21" s="41"/>
-      <c r="G21" s="41"/>
-      <c r="H21" s="41"/>
+      <c r="F21" s="49"/>
+      <c r="G21" s="49"/>
+      <c r="H21" s="49"/>
       <c r="I21" s="1"/>
       <c r="J21" s="2"/>
       <c r="K21" s="2"/>
@@ -3251,12 +3329,12 @@
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
-      <c r="E22" s="39" t="s">
+      <c r="E22" s="47" t="s">
         <v>168</v>
       </c>
-      <c r="F22" s="39"/>
-      <c r="G22" s="39"/>
-      <c r="H22" s="39"/>
+      <c r="F22" s="47"/>
+      <c r="G22" s="47"/>
+      <c r="H22" s="47"/>
       <c r="I22" s="1"/>
       <c r="J22" s="1"/>
       <c r="K22" s="1"/>
@@ -3897,7 +3975,7 @@
       <c r="A7" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="B7" s="42" t="s">
+      <c r="B7" s="39" t="s">
         <v>190</v>
       </c>
       <c r="C7" s="26"/>
@@ -3917,7 +3995,7 @@
       <c r="A8" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="B8" s="42" t="s">
+      <c r="B8" s="39" t="s">
         <v>365</v>
       </c>
       <c r="C8" s="26"/>
@@ -3937,7 +4015,7 @@
       <c r="A9" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="B9" s="42" t="s">
+      <c r="B9" s="39" t="s">
         <v>366</v>
       </c>
       <c r="C9" s="26"/>
@@ -3957,7 +4035,7 @@
       <c r="A10" s="4" t="s">
         <v>159</v>
       </c>
-      <c r="B10" s="43" t="s">
+      <c r="B10" s="40" t="s">
         <v>191</v>
       </c>
       <c r="C10" s="26"/>
@@ -3977,7 +4055,7 @@
       <c r="A11" s="4" t="s">
         <v>338</v>
       </c>
-      <c r="B11" s="43" t="s">
+      <c r="B11" s="40" t="s">
         <v>337</v>
       </c>
       <c r="C11" s="26"/>
@@ -3997,7 +4075,7 @@
       <c r="A12" s="4" t="s">
         <v>339</v>
       </c>
-      <c r="B12" s="43" t="s">
+      <c r="B12" s="40" t="s">
         <v>192</v>
       </c>
       <c r="C12" s="26"/>
@@ -4205,7 +4283,7 @@
       <c r="A20" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="B20" s="42" t="s">
+      <c r="B20" s="39" t="s">
         <v>190</v>
       </c>
       <c r="C20" s="26"/>
@@ -4225,7 +4303,7 @@
       <c r="A21" s="15" t="s">
         <v>58</v>
       </c>
-      <c r="B21" s="42" t="s">
+      <c r="B21" s="39" t="s">
         <v>365</v>
       </c>
       <c r="C21" s="26"/>
@@ -4245,7 +4323,7 @@
       <c r="A22" s="15" t="s">
         <v>59</v>
       </c>
-      <c r="B22" s="42" t="s">
+      <c r="B22" s="39" t="s">
         <v>366</v>
       </c>
       <c r="C22" s="26"/>
@@ -4265,7 +4343,7 @@
       <c r="A23" s="15" t="s">
         <v>159</v>
       </c>
-      <c r="B23" s="43" t="s">
+      <c r="B23" s="40" t="s">
         <v>369</v>
       </c>
       <c r="C23" s="26"/>
@@ -4285,7 +4363,7 @@
       <c r="A24" s="4" t="s">
         <v>338</v>
       </c>
-      <c r="B24" s="43" t="s">
+      <c r="B24" s="40" t="s">
         <v>370</v>
       </c>
       <c r="C24" s="26"/>
@@ -4305,7 +4383,7 @@
       <c r="A25" s="4" t="s">
         <v>339</v>
       </c>
-      <c r="B25" s="43" t="s">
+      <c r="B25" s="40" t="s">
         <v>192</v>
       </c>
       <c r="C25" s="26"/>
@@ -4585,7 +4663,7 @@
       <c r="A33" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="B33" s="42" t="s">
+      <c r="B33" s="39" t="s">
         <v>244</v>
       </c>
       <c r="C33" s="26" t="s">
@@ -4629,7 +4707,7 @@
       <c r="A34" s="15" t="s">
         <v>58</v>
       </c>
-      <c r="B34" s="42" t="s">
+      <c r="B34" s="39" t="s">
         <v>257</v>
       </c>
       <c r="C34" s="26" t="s">
@@ -4673,7 +4751,7 @@
       <c r="A35" s="15" t="s">
         <v>59</v>
       </c>
-      <c r="B35" s="42" t="s">
+      <c r="B35" s="39" t="s">
         <v>270</v>
       </c>
       <c r="C35" s="26" t="s">
@@ -4717,7 +4795,7 @@
       <c r="A36" s="15" t="s">
         <v>159</v>
       </c>
-      <c r="B36" s="43" t="s">
+      <c r="B36" s="40" t="s">
         <v>283</v>
       </c>
       <c r="C36" s="26" t="s">
@@ -4761,7 +4839,7 @@
       <c r="A37" s="4" t="s">
         <v>338</v>
       </c>
-      <c r="B37" s="43" t="s">
+      <c r="B37" s="40" t="s">
         <v>323</v>
       </c>
       <c r="C37" s="26" t="s">
@@ -4805,7 +4883,7 @@
       <c r="A38" s="4" t="s">
         <v>339</v>
       </c>
-      <c r="B38" s="43" t="s">
+      <c r="B38" s="40" t="s">
         <v>352</v>
       </c>
       <c r="C38" s="26" t="s">
@@ -4858,7 +4936,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47B91243-A115-4684-A5E9-C7F45B75B539}">
   <dimension ref="A1:L22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="N20" sqref="N20"/>
     </sheetView>
   </sheetViews>
@@ -4895,7 +4973,7 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="44" t="s">
+      <c r="A2" s="41" t="s">
         <v>41</v>
       </c>
       <c r="B2" s="14" t="s">
@@ -4947,7 +5025,7 @@
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="44" t="s">
+      <c r="A6" s="41" t="s">
         <v>41</v>
       </c>
       <c r="B6" s="3" t="s">
@@ -4986,7 +5064,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L25" sqref="L25"/>
+      <selection sqref="A1:B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5030,4 +5108,142 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB9FED9B-9F3E-4AD3-9299-A6818519B4B8}">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.28515625" customWidth="1"/>
+    <col min="2" max="2" width="31.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>371</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="21" x14ac:dyDescent="0.25">
+      <c r="A2" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>371</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="21" x14ac:dyDescent="0.25">
+      <c r="A5" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>373</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{559D6342-B60B-4CB6-BE35-7B783B0A93E0}">
+  <dimension ref="A1:E6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="5" width="20.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>378</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="80.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2" s="42" t="s">
+        <v>374</v>
+      </c>
+      <c r="C2" s="46" t="s">
+        <v>375</v>
+      </c>
+      <c r="D2" s="44" t="s">
+        <v>376</v>
+      </c>
+      <c r="E2" s="43" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>378</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="B6" s="45" t="s">
+        <v>379</v>
+      </c>
+      <c r="C6" s="45" t="s">
+        <v>380</v>
+      </c>
+      <c r="D6" s="45" t="s">
+        <v>381</v>
+      </c>
+      <c r="E6" s="45" t="s">
+        <v>382</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Se agrega función top defectos
</commit_message>
<xml_diff>
--- a/distribucion.xlsx
+++ b/distribucion.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Registro_defectos_SEHO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB2A5973-1D5A-4DB0-A362-F674D5C873EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E776637F-B99D-44EE-B02E-1DDBD0B91018}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="8" xr2:uid="{C5A581BF-84BA-4755-84C9-6391AAA71289}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{C5A581BF-84BA-4755-84C9-6391AAA71289}"/>
   </bookViews>
   <sheets>
     <sheet name="Frame0" sheetId="2" r:id="rId1"/>
@@ -80,7 +80,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="796" uniqueCount="465">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="800" uniqueCount="467">
   <si>
     <t>FA08</t>
   </si>
@@ -1475,6 +1475,12 @@
   </si>
   <si>
     <t>date_rd_1</t>
+  </si>
+  <si>
+    <t>button_17</t>
+  </si>
+  <si>
+    <t>Actualizar</t>
   </si>
 </sst>
 </file>
@@ -1850,7 +1856,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="77">
+  <cellXfs count="75">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2019,6 +2025,30 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="23" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="23" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="23" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2037,37 +2067,7 @@
     <xf numFmtId="0" fontId="5" fillId="25" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="23" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="23" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -4438,15 +4438,15 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6800F5CA-0E67-4275-894A-AE98A3C80F51}">
   <sheetPr codeName="Hoja4"/>
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
-    <sheetView zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>147</v>
       </c>
@@ -4471,8 +4471,11 @@
       <c r="H1" s="4" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I1" s="4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>41</v>
       </c>
@@ -4497,8 +4500,11 @@
       <c r="H2" s="14" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I2" s="3" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
         <v>147</v>
       </c>
@@ -4523,8 +4529,11 @@
       <c r="H4" s="4" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I4" s="4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>41</v>
       </c>
@@ -4548,6 +4557,9 @@
       </c>
       <c r="H5" s="14" t="s">
         <v>158</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>465</v>
       </c>
     </row>
   </sheetData>
@@ -4562,8 +4574,8 @@
   <sheetPr codeName="Hoja5"/>
   <dimension ref="A1:AC38"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="C38" sqref="C38:N38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5806,7 +5818,7 @@
   <dimension ref="A1:L22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N20" sqref="N20"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6120,40 +6132,40 @@
       <c r="A5" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="B5" s="75" t="s">
+      <c r="B5" s="14" t="s">
         <v>458</v>
       </c>
-      <c r="C5" s="75" t="s">
+      <c r="C5" s="14" t="s">
         <v>461</v>
       </c>
-      <c r="D5" s="75" t="s">
+      <c r="D5" s="14" t="s">
         <v>459</v>
       </c>
-      <c r="E5" s="76" t="s">
+      <c r="E5" s="52" t="s">
         <v>464</v>
       </c>
-      <c r="F5" s="75" t="s">
+      <c r="F5" s="14" t="s">
         <v>452</v>
       </c>
-      <c r="G5" s="75" t="s">
+      <c r="G5" s="14" t="s">
         <v>453</v>
       </c>
-      <c r="H5" s="75" t="s">
+      <c r="H5" s="14" t="s">
         <v>454</v>
       </c>
-      <c r="I5" s="75" t="s">
+      <c r="I5" s="14" t="s">
         <v>460</v>
       </c>
-      <c r="J5" s="75" t="s">
+      <c r="J5" s="14" t="s">
         <v>455</v>
       </c>
-      <c r="K5" s="75" t="s">
+      <c r="K5" s="14" t="s">
         <v>456</v>
       </c>
-      <c r="L5" s="75" t="s">
+      <c r="L5" s="14" t="s">
         <v>457</v>
       </c>
-      <c r="M5" s="75" t="s">
+      <c r="M5" s="14" t="s">
         <v>463</v>
       </c>
     </row>
@@ -6167,8 +6179,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E87CC77D-451D-4938-839F-1695B8C726C1}">
   <dimension ref="A1:W59"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K27" sqref="K27"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H35" sqref="H35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6177,117 +6189,117 @@
       <c r="A1" s="5" t="s">
         <v>376</v>
       </c>
-      <c r="B1" s="67" t="s">
+      <c r="B1" s="64" t="s">
         <v>42</v>
       </c>
-      <c r="C1" s="68"/>
-      <c r="D1" s="67" t="s">
+      <c r="C1" s="65"/>
+      <c r="D1" s="64" t="s">
         <v>43</v>
       </c>
-      <c r="E1" s="68"/>
-      <c r="F1" s="67" t="s">
+      <c r="E1" s="65"/>
+      <c r="F1" s="64" t="s">
         <v>44</v>
       </c>
-      <c r="G1" s="68"/>
+      <c r="G1" s="65"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="B2" s="66" t="s">
+      <c r="B2" s="60" t="s">
         <v>442</v>
       </c>
-      <c r="C2" s="66"/>
-      <c r="D2" s="66"/>
-      <c r="E2" s="66"/>
-      <c r="F2" s="66"/>
-      <c r="G2" s="66"/>
+      <c r="C2" s="60"/>
+      <c r="D2" s="60"/>
+      <c r="E2" s="60"/>
+      <c r="F2" s="60"/>
+      <c r="G2" s="60"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="B3" s="69" t="s">
+      <c r="B3" s="61" t="s">
         <v>449</v>
       </c>
-      <c r="C3" s="69"/>
-      <c r="D3" s="69" t="s">
+      <c r="C3" s="61"/>
+      <c r="D3" s="61" t="s">
         <v>450</v>
       </c>
-      <c r="E3" s="69"/>
-      <c r="F3" s="70" t="s">
+      <c r="E3" s="61"/>
+      <c r="F3" s="62" t="s">
         <v>451</v>
       </c>
-      <c r="G3" s="70"/>
+      <c r="G3" s="62"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="B4" s="71"/>
-      <c r="C4" s="72"/>
-      <c r="D4" s="71"/>
-      <c r="E4" s="72"/>
-      <c r="F4" s="71"/>
-      <c r="G4" s="72"/>
+      <c r="B4" s="66"/>
+      <c r="C4" s="67"/>
+      <c r="D4" s="66"/>
+      <c r="E4" s="67"/>
+      <c r="F4" s="66"/>
+      <c r="G4" s="67"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>376</v>
       </c>
-      <c r="B6" s="67" t="s">
+      <c r="B6" s="64" t="s">
         <v>42</v>
       </c>
-      <c r="C6" s="68"/>
-      <c r="D6" s="67" t="s">
+      <c r="C6" s="65"/>
+      <c r="D6" s="64" t="s">
         <v>43</v>
       </c>
-      <c r="E6" s="68"/>
-      <c r="F6" s="67" t="s">
+      <c r="E6" s="65"/>
+      <c r="F6" s="64" t="s">
         <v>44</v>
       </c>
-      <c r="G6" s="68"/>
+      <c r="G6" s="65"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="B7" s="66" t="s">
+      <c r="B7" s="60" t="s">
         <v>442</v>
       </c>
-      <c r="C7" s="66"/>
-      <c r="D7" s="66"/>
-      <c r="E7" s="66"/>
-      <c r="F7" s="66"/>
-      <c r="G7" s="66"/>
+      <c r="C7" s="60"/>
+      <c r="D7" s="60"/>
+      <c r="E7" s="60"/>
+      <c r="F7" s="60"/>
+      <c r="G7" s="60"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="B8" s="69" t="s">
+      <c r="B8" s="61" t="s">
         <v>449</v>
       </c>
-      <c r="C8" s="69"/>
-      <c r="D8" s="69" t="s">
+      <c r="C8" s="61"/>
+      <c r="D8" s="61" t="s">
         <v>450</v>
       </c>
-      <c r="E8" s="69"/>
-      <c r="F8" s="70" t="s">
+      <c r="E8" s="61"/>
+      <c r="F8" s="62" t="s">
         <v>441</v>
       </c>
-      <c r="G8" s="70"/>
+      <c r="G8" s="62"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="B9" s="73"/>
-      <c r="C9" s="73"/>
-      <c r="D9" s="73"/>
-      <c r="E9" s="73"/>
-      <c r="F9" s="73"/>
-      <c r="G9" s="73"/>
+      <c r="B9" s="63"/>
+      <c r="C9" s="63"/>
+      <c r="D9" s="63"/>
+      <c r="E9" s="63"/>
+      <c r="F9" s="63"/>
+      <c r="G9" s="63"/>
     </row>
     <row r="24" spans="2:23" x14ac:dyDescent="0.25">
       <c r="O24" s="54" t="s">
@@ -6305,10 +6317,10 @@
       <c r="S24" s="54" t="s">
         <v>441</v>
       </c>
-      <c r="T24" s="64" t="s">
+      <c r="T24" s="72" t="s">
         <v>446</v>
       </c>
-      <c r="U24" s="65"/>
+      <c r="U24" s="73"/>
       <c r="V24" s="54" t="s">
         <v>447</v>
       </c>
@@ -6324,8 +6336,8 @@
       <c r="Q25" s="55"/>
       <c r="R25" s="55"/>
       <c r="S25" s="55"/>
-      <c r="T25" s="60"/>
-      <c r="U25" s="61"/>
+      <c r="T25" s="68"/>
+      <c r="U25" s="69"/>
       <c r="V25" s="56"/>
       <c r="W25" s="56"/>
     </row>
@@ -6337,8 +6349,8 @@
       <c r="Q26" s="3"/>
       <c r="R26" s="3"/>
       <c r="S26" s="3"/>
-      <c r="T26" s="62"/>
-      <c r="U26" s="63"/>
+      <c r="T26" s="70"/>
+      <c r="U26" s="71"/>
       <c r="V26" s="17"/>
       <c r="W26" s="17"/>
     </row>
@@ -6350,8 +6362,8 @@
       <c r="Q27" s="55"/>
       <c r="R27" s="55"/>
       <c r="S27" s="55"/>
-      <c r="T27" s="60"/>
-      <c r="U27" s="61"/>
+      <c r="T27" s="68"/>
+      <c r="U27" s="69"/>
       <c r="V27" s="56"/>
       <c r="W27" s="56"/>
     </row>
@@ -6363,8 +6375,8 @@
       <c r="Q28" s="3"/>
       <c r="R28" s="3"/>
       <c r="S28" s="3"/>
-      <c r="T28" s="62"/>
-      <c r="U28" s="63"/>
+      <c r="T28" s="70"/>
+      <c r="U28" s="71"/>
       <c r="V28" s="17"/>
       <c r="W28" s="17"/>
     </row>
@@ -6382,8 +6394,8 @@
       <c r="Q29" s="55"/>
       <c r="R29" s="55"/>
       <c r="S29" s="55"/>
-      <c r="T29" s="60"/>
-      <c r="U29" s="61"/>
+      <c r="T29" s="68"/>
+      <c r="U29" s="69"/>
       <c r="V29" s="56"/>
       <c r="W29" s="56"/>
     </row>
@@ -6399,8 +6411,8 @@
       <c r="Q30" s="3"/>
       <c r="R30" s="3"/>
       <c r="S30" s="3"/>
-      <c r="T30" s="62"/>
-      <c r="U30" s="63"/>
+      <c r="T30" s="70"/>
+      <c r="U30" s="71"/>
       <c r="V30" s="17"/>
       <c r="W30" s="17"/>
     </row>
@@ -6416,8 +6428,8 @@
       <c r="Q31" s="55"/>
       <c r="R31" s="55"/>
       <c r="S31" s="55"/>
-      <c r="T31" s="60"/>
-      <c r="U31" s="61"/>
+      <c r="T31" s="68"/>
+      <c r="U31" s="69"/>
       <c r="V31" s="56"/>
       <c r="W31" s="56"/>
     </row>
@@ -6433,8 +6445,8 @@
       <c r="Q32" s="3"/>
       <c r="R32" s="3"/>
       <c r="S32" s="3"/>
-      <c r="T32" s="62"/>
-      <c r="U32" s="63"/>
+      <c r="T32" s="70"/>
+      <c r="U32" s="71"/>
       <c r="V32" s="17"/>
       <c r="W32" s="17"/>
     </row>
@@ -6450,8 +6462,8 @@
       <c r="Q33" s="55"/>
       <c r="R33" s="55"/>
       <c r="S33" s="55"/>
-      <c r="T33" s="60"/>
-      <c r="U33" s="61"/>
+      <c r="T33" s="68"/>
+      <c r="U33" s="69"/>
       <c r="V33" s="56"/>
       <c r="W33" s="56"/>
     </row>
@@ -6467,8 +6479,8 @@
       <c r="Q34" s="3"/>
       <c r="R34" s="3"/>
       <c r="S34" s="3"/>
-      <c r="T34" s="62"/>
-      <c r="U34" s="63"/>
+      <c r="T34" s="70"/>
+      <c r="U34" s="71"/>
       <c r="V34" s="17"/>
       <c r="W34" s="17"/>
     </row>
@@ -6624,13 +6636,17 @@
     </row>
   </sheetData>
   <mergeCells count="31">
-    <mergeCell ref="B7:G7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="F8:G8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="F9:G9"/>
+    <mergeCell ref="T33:U33"/>
+    <mergeCell ref="T34:U34"/>
+    <mergeCell ref="T24:U24"/>
+    <mergeCell ref="T25:U25"/>
+    <mergeCell ref="T26:U26"/>
+    <mergeCell ref="T27:U27"/>
+    <mergeCell ref="T28:U28"/>
+    <mergeCell ref="T29:U29"/>
+    <mergeCell ref="T32:U32"/>
+    <mergeCell ref="T30:U30"/>
+    <mergeCell ref="T31:U31"/>
     <mergeCell ref="B2:G2"/>
     <mergeCell ref="D1:E1"/>
     <mergeCell ref="F1:G1"/>
@@ -6644,17 +6660,13 @@
     <mergeCell ref="B4:C4"/>
     <mergeCell ref="D4:E4"/>
     <mergeCell ref="F4:G4"/>
-    <mergeCell ref="T33:U33"/>
-    <mergeCell ref="T34:U34"/>
-    <mergeCell ref="T24:U24"/>
-    <mergeCell ref="T25:U25"/>
-    <mergeCell ref="T26:U26"/>
-    <mergeCell ref="T27:U27"/>
-    <mergeCell ref="T28:U28"/>
-    <mergeCell ref="T29:U29"/>
-    <mergeCell ref="T32:U32"/>
-    <mergeCell ref="T30:U30"/>
-    <mergeCell ref="T31:U31"/>
+    <mergeCell ref="B7:G7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="F9:G9"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>